<commit_message>
Updated sgd, main script --> script_1.m
</commit_message>
<xml_diff>
--- a/code/toy_movies.xlsx
+++ b/code/toy_movies.xlsx
@@ -5,15 +5,18 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeken/Dropbox/462/project/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oeken/Dropbox/462/cathar/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="19620" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="full_toy" sheetId="1" r:id="rId1"/>
+    <sheet name="half_toy" sheetId="2" r:id="rId2"/>
+    <sheet name="recom" sheetId="6" r:id="rId3"/>
+    <sheet name="reel_est" sheetId="5" r:id="rId4"/>
+    <sheet name="l_vs_reg_vs_err" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="331">
   <si>
     <t>The Imitation Game</t>
   </si>
@@ -154,15 +157,886 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>Liked</t>
+  </si>
+  <si>
+    <t>Disliked</t>
+  </si>
+  <si>
+    <t>Reel</t>
+  </si>
+  <si>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.90          0.91          0.92          0.93          0.94          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.88          0.90          0.92          0.93          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.88          0.90          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.87          0.90          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.83          0.89          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.81          0.89          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.78          0.89          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.76          0.88          0.91          0.92          0.93          0.94          0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.96          0.96          0.97          0.97          0.98          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.96          0.96          0.96          0.97          0.98          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.96          0.96          0.96          0.97          0.97          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.96          0.96          0.97          0.98          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.96          0.96          0.97          0.97          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.96          0.96          0.97          0.97          0.98          0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.99          0.96          0.96          0.97          0.97          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.98          0.96          0.96          0.97          0.97          0.98          0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.99          0.96          0.96          0.97          0.97          0.98          0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          1.00          0.96          0.96          0.97          0.97          0.98          0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.92          0.93          0.95          0.98          1.01          1.06          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.92          0.93          0.94          0.97          1.01          1.05          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.90          0.92          0.94          0.97          1.00          1.06          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.90          0.92          0.94          0.97          1.01          1.05          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.89          0.92          0.94          0.97          1.00          1.05          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.88          0.91          0.94          0.97          1.01          1.05          1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.87          0.91          0.94          0.97          1.00          1.05          1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.86          0.91          0.94          0.97          1.01          1.05          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.82          0.90          0.94          0.97          1.01          1.04          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.77          0.90          0.93          0.96          1.00          1.05          1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.98          0.99          1.02          1.05          1.09          1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.97          0.99          1.01          1.05          1.09          1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.97          0.99          1.01          1.04          1.09          1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.97          0.99          1.01          1.05          1.08          1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.97          0.97          0.99          1.00          1.04          1.09          1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.98          0.97          0.98          1.01          1.04          1.08          1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.98          0.97          0.99          1.01          1.04          1.09          1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.98          0.97          0.98          1.01          1.04          1.08          1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          0.99          0.97          0.98          1.01          1.04          1.08          1.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          1.00          0.97          0.98          1.00          1.04          1.08          1.14</t>
+  </si>
+  <si>
+    <t>BIAS ON</t>
+  </si>
+  <si>
+    <t>BIAS OFF</t>
+  </si>
+  <si>
+    <t>RMS Error on Test Data</t>
+  </si>
+  <si>
+    <t>RMS Error on Training Data</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>1.06</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>1.04</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>1.09</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>'Babe (1995)'</t>
+  </si>
+  <si>
+    <t>'Muppet Treasure Island (1996)'</t>
+  </si>
+  <si>
+    <t>'Batman Forever (1995)'</t>
+  </si>
+  <si>
+    <t>'Free Willy 2: The Adventure Home (1995)'</t>
+  </si>
+  <si>
+    <t>'Operation Dumbo Drop (1995)'</t>
+  </si>
+  <si>
+    <t>'Breakfast at Tiffany''s (1961)'</t>
+  </si>
+  <si>
+    <t>'D3: The Mighty Ducks (1996)'</t>
+  </si>
+  <si>
+    <t>'Batman Returns (1992)'</t>
+  </si>
+  <si>
+    <t>'Turbo: A Power Rangers Movie (1997)'</t>
+  </si>
+  <si>
+    <t>'Air Bud (1997)'</t>
+  </si>
+  <si>
+    <t>'Steel (1997)'</t>
+  </si>
+  <si>
+    <t>Known Disliked</t>
+  </si>
+  <si>
+    <t>Known Liked</t>
+  </si>
+  <si>
+    <t>'Toy Story (1995)'</t>
+  </si>
+  <si>
+    <t>'Dead Man Walking (1995)'</t>
+  </si>
+  <si>
+    <t>'Mighty Aphrodite (1995)'</t>
+  </si>
+  <si>
+    <t>'Mr. Holland''s Opus (1995)'</t>
+  </si>
+  <si>
+    <t>'French Twist (Gazon maudit) (1995)'</t>
+  </si>
+  <si>
+    <t>'Antonia''s Line (1995)'</t>
+  </si>
+  <si>
+    <t>'Crumb (1994)'</t>
+  </si>
+  <si>
+    <t>'Clerks (1994)'</t>
+  </si>
+  <si>
+    <t>'Eat Drink Man Woman (1994)'</t>
+  </si>
+  <si>
+    <t>'Hoop Dreams (1994)'</t>
+  </si>
+  <si>
+    <t>'Star Wars (1977)'</t>
+  </si>
+  <si>
+    <t>'Professional, The (1994)'</t>
+  </si>
+  <si>
+    <t>'Priest (1994)'</t>
+  </si>
+  <si>
+    <t>'Three Colors: Red (1994)'</t>
+  </si>
+  <si>
+    <t>'Searching for Bobby Fischer (1993)'</t>
+  </si>
+  <si>
+    <t>'Blade Runner (1982)'</t>
+  </si>
+  <si>
+    <t>'Welcome to the Dollhouse (1995)'</t>
+  </si>
+  <si>
+    <t>'Mystery Science Theater 3000: The Movie (1996)'</t>
+  </si>
+  <si>
+    <t>'Truth About Cats &amp; Dogs, The (1996)'</t>
+  </si>
+  <si>
+    <t>'Haunted World of Edward D. Wood Jr., The (1995)'</t>
+  </si>
+  <si>
+    <t>'Maya Lin: A Strong Clear Vision (1994)'</t>
+  </si>
+  <si>
+    <t>'Lone Star (1996)'</t>
+  </si>
+  <si>
+    <t>'Godfather, The (1972)'</t>
+  </si>
+  <si>
+    <t>'Big Night (1996)'</t>
+  </si>
+  <si>
+    <t>'Sleeper (1973)'</t>
+  </si>
+  <si>
+    <t>'Jean de Florette (1986)'</t>
+  </si>
+  <si>
+    <t>'Manon of the Spring (Manon des sources) (1986)'</t>
+  </si>
+  <si>
+    <t>'Monty Python and the Holy Grail (1974)'</t>
+  </si>
+  <si>
+    <t>'Wrong Trousers, The (1993)'</t>
+  </si>
+  <si>
+    <t>'Empire Strikes Back, The (1980)'</t>
+  </si>
+  <si>
+    <t>'Princess Bride, The (1987)'</t>
+  </si>
+  <si>
+    <t>'Aliens (1986)'</t>
+  </si>
+  <si>
+    <t>'12 Angry Men (1957)'</t>
+  </si>
+  <si>
+    <t>'Return of the Jedi (1983)'</t>
+  </si>
+  <si>
+    <t>'Amadeus (1984)'</t>
+  </si>
+  <si>
+    <t>'Terminator, The (1984)'</t>
+  </si>
+  <si>
+    <t>'Graduate, The (1967)'</t>
+  </si>
+  <si>
+    <t>'Nikita (La Femme Nikita) (1990)'</t>
+  </si>
+  <si>
+    <t>'Back to the Future (1985)'</t>
+  </si>
+  <si>
+    <t>'Cyrano de Bergerac (1990)'</t>
+  </si>
+  <si>
+    <t>'When Harry Met Sally... (1989)'</t>
+  </si>
+  <si>
+    <t>'Sling Blade (1996)'</t>
+  </si>
+  <si>
+    <t>'Chasing Amy (1997)'</t>
+  </si>
+  <si>
+    <t>'Full Monty, The (1997)'</t>
+  </si>
+  <si>
+    <t>'Gattaca (1997)'</t>
+  </si>
+  <si>
+    <t>Unknown Disliked</t>
+  </si>
+  <si>
+    <t>'Faster Pussycat! Kill! Kill! (1965)'</t>
+  </si>
+  <si>
+    <t>'Free Willy (1993)'</t>
+  </si>
+  <si>
+    <t>'All Dogs Go to Heaven 2 (1996)'</t>
+  </si>
+  <si>
+    <t>'Theodore Rex (1995)'</t>
+  </si>
+  <si>
+    <t>'Flipper (1996)'</t>
+  </si>
+  <si>
+    <t>'Striptease (1996)'</t>
+  </si>
+  <si>
+    <t>'Homeward Bound: The Incredible Journey (1993)'</t>
+  </si>
+  <si>
+    <t>'Sound of Music, The (1965)'</t>
+  </si>
+  <si>
+    <t>'Nightmare on Elm Street, A (1984)'</t>
+  </si>
+  <si>
+    <t>'Jungle2Jungle (1997)'</t>
+  </si>
+  <si>
+    <t>'Batman &amp; Robin (1997)'</t>
+  </si>
+  <si>
+    <t>'George of the Jungle (1997)'</t>
+  </si>
+  <si>
+    <t>'Event Horizon (1997)'</t>
+  </si>
+  <si>
+    <t>'Kull the Conqueror (1997)'</t>
+  </si>
+  <si>
+    <t>'Shanghai Triad (Yao a yao yao dao waipo qiao) (1995)'</t>
+  </si>
+  <si>
+    <t>'Usual Suspects, The (1995)'</t>
+  </si>
+  <si>
+    <t>'Postino, Il (1994)'</t>
+  </si>
+  <si>
+    <t>'Dolores Claiborne (1994)'</t>
+  </si>
+  <si>
+    <t>'Three Colors: Blue (1993)'</t>
+  </si>
+  <si>
+    <t>'Shawshank Redemption, The (1994)'</t>
+  </si>
+  <si>
+    <t>'Hudsucker Proxy, The (1994)'</t>
+  </si>
+  <si>
+    <t>'Jurassic Park (1993)'</t>
+  </si>
+  <si>
+    <t>'Remains of the Day, The (1993)'</t>
+  </si>
+  <si>
+    <t>'Nightmare Before Christmas, The (1993)'</t>
+  </si>
+  <si>
+    <t>'Terminator 2: Judgment Day (1991)'</t>
+  </si>
+  <si>
+    <t>'Fargo (1996)'</t>
+  </si>
+  <si>
+    <t>'Kids in the Hall: Brain Candy (1996)'</t>
+  </si>
+  <si>
+    <t>'Horseman on the Roof, The (Hussard sur le toit, Le) (1995)'</t>
+  </si>
+  <si>
+    <t>'Wallace &amp; Gromit: The Best of Aardman Animation (1996)'</t>
+  </si>
+  <si>
+    <t>'Bound (1996)'</t>
+  </si>
+  <si>
+    <t>'Swingers (1996)'</t>
+  </si>
+  <si>
+    <t>'Monty Python''s Life of Brian (1979)'</t>
+  </si>
+  <si>
+    <t>'Cinema Paradiso (1988)'</t>
+  </si>
+  <si>
+    <t>'Delicatessen (1991)'</t>
+  </si>
+  <si>
+    <t>'Raiders of the Lost Ark (1981)'</t>
+  </si>
+  <si>
+    <t>'Brazil (1985)'</t>
+  </si>
+  <si>
+    <t>'Good, The Bad and The Ugly, The (1966)'</t>
+  </si>
+  <si>
+    <t>'Alien (1979)'</t>
+  </si>
+  <si>
+    <t>'Henry V (1989)'</t>
+  </si>
+  <si>
+    <t>'Dead Poets Society (1989)'</t>
+  </si>
+  <si>
+    <t>'Groundhog Day (1993)'</t>
+  </si>
+  <si>
+    <t>'Young Frankenstein (1974)'</t>
+  </si>
+  <si>
+    <t>'Breaking the Waves (1996)'</t>
+  </si>
+  <si>
+    <t>'Ridicule (1996)'</t>
+  </si>
+  <si>
+    <t>'Star Trek: The Wrath of Khan (1982)'</t>
+  </si>
+  <si>
+    <t>'Mars Attacks! (1996)'</t>
+  </si>
+  <si>
+    <t>'Kolya (1996)'</t>
+  </si>
+  <si>
+    <t>'Pillow Book, The (1995)'</t>
+  </si>
+  <si>
+    <t>'Contact (1997)'</t>
+  </si>
+  <si>
+    <t>Recommended</t>
+  </si>
+  <si>
+    <t>Unrecommended</t>
+  </si>
+  <si>
+    <t>'Pather Panchali (1955)'</t>
+  </si>
+  <si>
+    <t>'Silence of the Lambs, The (1991)'</t>
+  </si>
+  <si>
+    <t>'Pulp Fiction (1994)'</t>
+  </si>
+  <si>
+    <t>'Schindler''s List (1993)'</t>
+  </si>
+  <si>
+    <t>'Saint of Fort Washington, The (1993)'</t>
+  </si>
+  <si>
+    <t>'Yankee Zulu (1994)'</t>
+  </si>
+  <si>
+    <t>'Psycho (1960)'</t>
+  </si>
+  <si>
+    <t>'Close Shave, A (1995)'</t>
+  </si>
+  <si>
+    <t>'High Noon (1952)'</t>
+  </si>
+  <si>
+    <t>'Apocalypse Now (1979)'</t>
+  </si>
+  <si>
+    <t>'One Flew Over the Cuckoo''s Nest (1975)'</t>
+  </si>
+  <si>
+    <t>'Aiqing wansui (1994)'</t>
+  </si>
+  <si>
+    <t>'Rear Window (1954)'</t>
+  </si>
+  <si>
+    <t>'Paradise Lost: The Child Murders at Robin Hood Hills (1996)'</t>
+  </si>
+  <si>
+    <t>'Citizen Kane (1941)'</t>
+  </si>
+  <si>
+    <t>'Dr. Strangelove or: How I Learned to Stop Worrying and Love the Bomb (1963)'</t>
+  </si>
+  <si>
+    <t>'Crossfire (1947)'</t>
+  </si>
+  <si>
+    <t>'Damsel in Distress, A (1937)'</t>
+  </si>
+  <si>
+    <t>'Some Mother''s Son (1996)'</t>
+  </si>
+  <si>
+    <t>'Casablanca (1942)'</t>
+  </si>
+  <si>
+    <t>'Lady of Burlesque (1943)'</t>
+  </si>
+  <si>
+    <t>'North by Northwest (1959)'</t>
+  </si>
+  <si>
+    <t>'Good Will Hunting (1997)'</t>
+  </si>
+  <si>
+    <t>'When We Were Kings (1996)'</t>
+  </si>
+  <si>
+    <t>'Boot, Das (1981)'</t>
+  </si>
+  <si>
+    <t>'Paris Was a Woman (1995)'</t>
+  </si>
+  <si>
+    <t>'Butcher Boy, The (1998)'</t>
+  </si>
+  <si>
+    <t>'Some Folks Call It a Sling Blade (1993)'</t>
+  </si>
+  <si>
+    <t>'Taxi Driver (1976)'</t>
+  </si>
+  <si>
+    <t>'Big Bang Theory, The (1994)'</t>
+  </si>
+  <si>
+    <t>'Sunset Blvd. (1950)'</t>
+  </si>
+  <si>
+    <t>'39 Steps, The (1935)'</t>
+  </si>
+  <si>
+    <t>'Paths of Glory (1957)'</t>
+  </si>
+  <si>
+    <t>'Wild Bunch, The (1969)'</t>
+  </si>
+  <si>
+    <t>'As Good As It Gets (1997)'</t>
+  </si>
+  <si>
+    <t>'Duck Soup (1933)'</t>
+  </si>
+  <si>
+    <t>'L.A. Confidential (1997)'</t>
+  </si>
+  <si>
+    <t>'Thin Man, The (1934)'</t>
+  </si>
+  <si>
+    <t>'Bitter Sugar (Azucar Amargo) (1996)'</t>
+  </si>
+  <si>
+    <t>'Braindead (1992)'</t>
+  </si>
+  <si>
+    <t>'Cool Hand Luke (1967)'</t>
+  </si>
+  <si>
+    <t>'His Girl Friday (1940)'</t>
+  </si>
+  <si>
+    <t>'Marlene Dietrich: Shadow and Light (1996)'</t>
+  </si>
+  <si>
+    <t>'Once Upon a Time in the West (1969)'</t>
+  </si>
+  <si>
+    <t>'Kazaam (1996)'</t>
+  </si>
+  <si>
+    <t>'Island of Dr. Moreau, The (1996)'</t>
+  </si>
+  <si>
+    <t>'Celtic Pride (1996)'</t>
+  </si>
+  <si>
+    <t>'Spy Hard (1996)'</t>
+  </si>
+  <si>
+    <t>'Cabin Boy (1994)'</t>
+  </si>
+  <si>
+    <t>'Meet Wally Sparks (1997)'</t>
+  </si>
+  <si>
+    <t>'Amityville 3-D (1983)'</t>
+  </si>
+  <si>
+    <t>'Drop Dead Fred (1991)'</t>
+  </si>
+  <si>
+    <t>'Man of the House (1995)'</t>
+  </si>
+  <si>
+    <t>'Leave It to Beaver (1997)'</t>
+  </si>
+  <si>
+    <t>'Dangerous Ground (1997)'</t>
+  </si>
+  <si>
+    <t>'Vampire in Brooklyn (1995)'</t>
+  </si>
+  <si>
+    <t>'Sunset Park (1996)'</t>
+  </si>
+  <si>
+    <t>'Beautician and the Beast, The (1997)'</t>
+  </si>
+  <si>
+    <t>'Amityville Curse, The (1990)'</t>
+  </si>
+  <si>
+    <t>'Gordy (1995)'</t>
+  </si>
+  <si>
+    <t>'Ed (1996)'</t>
+  </si>
+  <si>
+    <t>'That Darn Cat! (1997)'</t>
+  </si>
+  <si>
+    <t>'Super Mario Bros. (1993)'</t>
+  </si>
+  <si>
+    <t>'Anaconda (1997)'</t>
+  </si>
+  <si>
+    <t>'Wishmaster (1997)'</t>
+  </si>
+  <si>
+    <t>'Keys to Tulsa (1997)'</t>
+  </si>
+  <si>
+    <t>'White Man''s Burden (1995)'</t>
+  </si>
+  <si>
+    <t>'Pocahontas (1995)'</t>
+  </si>
+  <si>
+    <t>'Mortal Kombat: Annihilation (1997)'</t>
+  </si>
+  <si>
+    <t>'Lawnmower Man 2: Beyond Cyberspace (1996)'</t>
+  </si>
+  <si>
+    <t>'Land Before Time III: The Time of the Great Giving (1995) (V)'</t>
+  </si>
+  <si>
+    <t>'Jury Duty (1995)'</t>
+  </si>
+  <si>
+    <t>'Double Team (1997)'</t>
+  </si>
+  <si>
+    <t>'Big Bully (1996)'</t>
+  </si>
+  <si>
+    <t>'Poison Ivy II (1995)'</t>
+  </si>
+  <si>
+    <t>'Jingle All the Way (1996)'</t>
+  </si>
+  <si>
+    <t>'Ready to Wear (Pret-A-Porter) (1994)'</t>
+  </si>
+  <si>
+    <t>'Richie Rich (1994)'</t>
+  </si>
+  <si>
+    <t>'Getting Even with Dad (1994)'</t>
+  </si>
+  <si>
+    <t>'In the Army Now (1994)'</t>
+  </si>
+  <si>
+    <t>'Speed 2: Cruise Control (1997)'</t>
+  </si>
+  <si>
+    <t>'Amityville 1992: It''s About Time (1992)'</t>
+  </si>
+  <si>
+    <t>'B*A*P*S (1997)'</t>
+  </si>
+  <si>
+    <t>'Stupids, The (1996)'</t>
+  </si>
+  <si>
+    <t>'Amityville II: The Possession (1982)'</t>
+  </si>
+  <si>
+    <t>'Congo (1995)'</t>
+  </si>
+  <si>
+    <t>'Free Willy 3: The Rescue (1997)'</t>
+  </si>
+  <si>
+    <t>'Grease 2 (1982)'</t>
+  </si>
+  <si>
+    <t>'Children of the Corn: The Gathering (1996)'</t>
+  </si>
+  <si>
+    <t>'Solo (1996)'</t>
+  </si>
+  <si>
+    <t>'Bio-Dome (1996)'</t>
+  </si>
+  <si>
+    <t>Unknown Liked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -196,16 +1070,169 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -213,30 +1240,588 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="8" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="28" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="29" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="25" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="27" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="5" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="4" borderId="5" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="4" borderId="5" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="4" borderId="32" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="4" borderId="32" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="34" xfId="10" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="20% - Accent5" xfId="11" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="9" builtinId="31"/>
+    <cellStyle name="40% - Accent5" xfId="12" builtinId="47"/>
+    <cellStyle name="Accent3" xfId="10" builtinId="37"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="7" builtinId="22"/>
+    <cellStyle name="Explanatory Text" xfId="8" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="6" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2049,7 +3634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3551,4 +5136,2670 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:J57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.1640625" customWidth="1"/>
+    <col min="9" max="9" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:10" s="44" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="46" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" s="46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="J12" s="46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>290</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>247</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="J16" s="46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="J17" s="46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="J18" s="46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>251</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="J19" s="45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="J20" s="45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>254</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="J23" s="45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>256</v>
+      </c>
+      <c r="J24" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="46" t="s">
+        <v>300</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="46" t="s">
+        <v>302</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="J27" s="45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="J29" s="45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="46" t="s">
+        <v>305</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="J30" s="45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="J31" s="45" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="J32" s="45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="J33" s="45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="46" t="s">
+        <v>309</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="J34" s="45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="J35" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="J36" s="45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="J37" s="45" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>268</v>
+      </c>
+      <c r="J38" s="45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>269</v>
+      </c>
+      <c r="J39" s="45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="J40" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>271</v>
+      </c>
+      <c r="J42" s="45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="J43" s="45" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="D44" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="J44" s="45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="46" t="s">
+        <v>320</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="J45" s="45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="46" t="s">
+        <v>321</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="J46" s="45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="J47" s="45" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="J48" s="45" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B49" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="D49" s="46" t="s">
+        <v>276</v>
+      </c>
+      <c r="J49" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="J50" s="45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51" s="46" t="s">
+        <v>326</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B52" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B53" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="D53" s="46" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="D55" s="46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="2:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AL8"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="38" width="4.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:38" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="37">
+        <v>6</v>
+      </c>
+      <c r="E3" s="33">
+        <v>12</v>
+      </c>
+      <c r="F3" s="33">
+        <v>14</v>
+      </c>
+      <c r="G3" s="33">
+        <v>44</v>
+      </c>
+      <c r="H3" s="33">
+        <v>60</v>
+      </c>
+      <c r="I3" s="33">
+        <v>64</v>
+      </c>
+      <c r="J3" s="33">
+        <v>81</v>
+      </c>
+      <c r="K3" s="33">
+        <v>82</v>
+      </c>
+      <c r="L3" s="33">
+        <v>86</v>
+      </c>
+      <c r="M3" s="33">
+        <v>91</v>
+      </c>
+      <c r="N3" s="33">
+        <v>96</v>
+      </c>
+      <c r="O3" s="33">
+        <v>100</v>
+      </c>
+      <c r="P3" s="33">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="33">
+        <v>113</v>
+      </c>
+      <c r="R3" s="33">
+        <v>114</v>
+      </c>
+      <c r="S3" s="33">
+        <v>129</v>
+      </c>
+      <c r="T3" s="33">
+        <v>150</v>
+      </c>
+      <c r="U3" s="33">
+        <v>154</v>
+      </c>
+      <c r="V3" s="33">
+        <v>170</v>
+      </c>
+      <c r="W3" s="33">
+        <v>171</v>
+      </c>
+      <c r="X3" s="33">
+        <v>174</v>
+      </c>
+      <c r="Y3" s="33">
+        <v>175</v>
+      </c>
+      <c r="Z3" s="33">
+        <v>177</v>
+      </c>
+      <c r="AA3" s="33">
+        <v>183</v>
+      </c>
+      <c r="AB3" s="33">
+        <v>190</v>
+      </c>
+      <c r="AC3" s="33">
+        <v>196</v>
+      </c>
+      <c r="AD3" s="33">
+        <v>202</v>
+      </c>
+      <c r="AE3" s="33">
+        <v>208</v>
+      </c>
+      <c r="AF3" s="33">
+        <v>221</v>
+      </c>
+      <c r="AG3" s="33">
+        <v>224</v>
+      </c>
+      <c r="AH3" s="33">
+        <v>228</v>
+      </c>
+      <c r="AI3" s="33">
+        <v>235</v>
+      </c>
+      <c r="AJ3" s="33">
+        <v>242</v>
+      </c>
+      <c r="AK3" s="33">
+        <v>253</v>
+      </c>
+      <c r="AL3" s="33">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41"/>
+      <c r="C4" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="37">
+        <v>74</v>
+      </c>
+      <c r="E4" s="33">
+        <v>78</v>
+      </c>
+      <c r="F4" s="33">
+        <v>103</v>
+      </c>
+      <c r="G4" s="33">
+        <v>104</v>
+      </c>
+      <c r="H4" s="33">
+        <v>112</v>
+      </c>
+      <c r="I4" s="33">
+        <v>120</v>
+      </c>
+      <c r="J4" s="33">
+        <v>140</v>
+      </c>
+      <c r="K4" s="33">
+        <v>143</v>
+      </c>
+      <c r="L4" s="33">
+        <v>219</v>
+      </c>
+      <c r="M4" s="33">
+        <v>243</v>
+      </c>
+      <c r="N4" s="33">
+        <v>254</v>
+      </c>
+      <c r="O4" s="33">
+        <v>259</v>
+      </c>
+      <c r="P4" s="33">
+        <v>260</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>266</v>
+      </c>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="33"/>
+      <c r="AJ4" s="33"/>
+      <c r="AK4" s="33"/>
+      <c r="AL4" s="33"/>
+    </row>
+    <row r="5" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="37">
+        <v>5</v>
+      </c>
+      <c r="E5" s="33">
+        <v>5</v>
+      </c>
+      <c r="F5" s="33">
+        <v>5</v>
+      </c>
+      <c r="G5" s="33">
+        <v>5</v>
+      </c>
+      <c r="H5" s="33">
+        <v>5</v>
+      </c>
+      <c r="I5" s="33">
+        <v>5</v>
+      </c>
+      <c r="J5" s="33">
+        <v>5</v>
+      </c>
+      <c r="K5" s="33">
+        <v>5</v>
+      </c>
+      <c r="L5" s="33">
+        <v>5</v>
+      </c>
+      <c r="M5" s="33">
+        <v>5</v>
+      </c>
+      <c r="N5" s="33">
+        <v>5</v>
+      </c>
+      <c r="O5" s="33">
+        <v>5</v>
+      </c>
+      <c r="P5" s="33">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="33">
+        <v>5</v>
+      </c>
+      <c r="R5" s="33">
+        <v>5</v>
+      </c>
+      <c r="S5" s="33">
+        <v>5</v>
+      </c>
+      <c r="T5" s="33">
+        <v>5</v>
+      </c>
+      <c r="U5" s="33">
+        <v>5</v>
+      </c>
+      <c r="V5" s="33">
+        <v>5</v>
+      </c>
+      <c r="W5" s="33">
+        <v>5</v>
+      </c>
+      <c r="X5" s="33">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="33">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AE5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AG5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AJ5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="33">
+        <v>5</v>
+      </c>
+      <c r="AL5" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="41"/>
+      <c r="C6" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="37">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1</v>
+      </c>
+      <c r="I6" s="33">
+        <v>1</v>
+      </c>
+      <c r="J6" s="33">
+        <v>1</v>
+      </c>
+      <c r="K6" s="33">
+        <v>1</v>
+      </c>
+      <c r="L6" s="33">
+        <v>1</v>
+      </c>
+      <c r="M6" s="33">
+        <v>1</v>
+      </c>
+      <c r="N6" s="33">
+        <v>1</v>
+      </c>
+      <c r="O6" s="33">
+        <v>1</v>
+      </c>
+      <c r="P6" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="33">
+        <v>1</v>
+      </c>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33"/>
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="33"/>
+      <c r="AF6" s="33"/>
+      <c r="AG6" s="33"/>
+      <c r="AH6" s="33"/>
+      <c r="AI6" s="33"/>
+      <c r="AJ6" s="33"/>
+      <c r="AK6" s="33"/>
+      <c r="AL6" s="33"/>
+    </row>
+    <row r="7" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="38">
+        <v>3.8099999000000002</v>
+      </c>
+      <c r="E7" s="34">
+        <v>4.7600002000000003</v>
+      </c>
+      <c r="F7" s="34">
+        <v>4.3899999000000003</v>
+      </c>
+      <c r="G7" s="34">
+        <v>3.1900000999999998</v>
+      </c>
+      <c r="H7" s="34">
+        <v>4.7800001999999999</v>
+      </c>
+      <c r="I7" s="34">
+        <v>4.6100000999999997</v>
+      </c>
+      <c r="J7" s="34">
+        <v>3.8599999</v>
+      </c>
+      <c r="K7" s="34">
+        <v>3.2</v>
+      </c>
+      <c r="L7" s="34">
+        <v>4.3400002000000004</v>
+      </c>
+      <c r="M7" s="34">
+        <v>3.8699998999999998</v>
+      </c>
+      <c r="N7" s="34">
+        <v>3.9400000999999998</v>
+      </c>
+      <c r="O7" s="34">
+        <v>4.75</v>
+      </c>
+      <c r="P7" s="34">
+        <v>3.4200001000000002</v>
+      </c>
+      <c r="Q7" s="34">
+        <v>4.0900002000000004</v>
+      </c>
+      <c r="R7" s="34">
+        <v>4.5</v>
+      </c>
+      <c r="S7" s="34">
+        <v>4.1599997999999996</v>
+      </c>
+      <c r="T7" s="34">
+        <v>4.1999997999999996</v>
+      </c>
+      <c r="U7" s="34">
+        <v>4.4099997999999996</v>
+      </c>
+      <c r="V7" s="34">
+        <v>4.1700001000000002</v>
+      </c>
+      <c r="W7" s="34">
+        <v>4.54</v>
+      </c>
+      <c r="X7" s="34">
+        <v>4.2199998000000001</v>
+      </c>
+      <c r="Y7" s="34">
+        <v>4.4699998000000001</v>
+      </c>
+      <c r="Z7" s="34">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="AA7" s="34">
+        <v>4.6100000999999997</v>
+      </c>
+      <c r="AB7" s="34">
+        <v>4.4899997999999997</v>
+      </c>
+      <c r="AC7" s="34">
+        <v>3.96</v>
+      </c>
+      <c r="AD7" s="34">
+        <v>3.8800001000000002</v>
+      </c>
+      <c r="AE7" s="34">
+        <v>4.1300001000000002</v>
+      </c>
+      <c r="AF7" s="34">
+        <v>4.0100002000000003</v>
+      </c>
+      <c r="AG7" s="34">
+        <v>4.0300001999999999</v>
+      </c>
+      <c r="AH7" s="34">
+        <v>3.8199999</v>
+      </c>
+      <c r="AI7" s="34">
+        <v>3.05</v>
+      </c>
+      <c r="AJ7" s="34">
+        <v>4.5500002000000004</v>
+      </c>
+      <c r="AK7" s="34">
+        <v>4.0700002</v>
+      </c>
+      <c r="AL7" s="34">
+        <v>4.0500002000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="41"/>
+      <c r="C8" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="39">
+        <v>3.6442768674136601</v>
+      </c>
+      <c r="E8" s="35">
+        <v>1.44828568491678</v>
+      </c>
+      <c r="F8" s="35">
+        <v>2.0758800756937097</v>
+      </c>
+      <c r="G8" s="35">
+        <v>2.26196612832626</v>
+      </c>
+      <c r="H8" s="35">
+        <v>1.7247213697510801</v>
+      </c>
+      <c r="I8" s="35">
+        <v>1.8364572079421599</v>
+      </c>
+      <c r="J8" s="35">
+        <v>2.80204489291068</v>
+      </c>
+      <c r="K8" s="35">
+        <v>3.6118767304380199</v>
+      </c>
+      <c r="L8" s="35">
+        <v>3.26570858683993</v>
+      </c>
+      <c r="M8" s="35">
+        <v>1.77904143434952</v>
+      </c>
+      <c r="N8" s="35">
+        <v>1.8616034103921202</v>
+      </c>
+      <c r="O8" s="35">
+        <v>2.2195190662420998</v>
+      </c>
+      <c r="P8" s="35">
+        <v>2.3970838513633401</v>
+      </c>
+      <c r="Q8" s="35">
+        <v>2.6638468795596002</v>
+      </c>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="36"/>
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="36"/>
+      <c r="AI8" s="36"/>
+      <c r="AJ8" s="36"/>
+      <c r="AK8" s="36"/>
+      <c r="AL8" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:R73"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="6" style="6" customWidth="1"/>
+    <col min="3" max="10" width="7.1640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" style="6" customWidth="1"/>
+    <col min="12" max="18" width="7.1640625" style="6" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
+      <c r="L2" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="32"/>
+    </row>
+    <row r="3" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="21">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4" s="23"/>
+      <c r="L4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="25"/>
+      <c r="C5" s="21">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="21">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="21">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="L7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="21">
+        <v>5</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="23"/>
+      <c r="L8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="21">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="21">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="21">
+        <v>8</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="21">
+        <v>9</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="21">
+        <v>10</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="R13" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+    </row>
+    <row r="15" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="21">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="21">
+        <v>2</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" s="23"/>
+      <c r="L16" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
+      <c r="C17" s="21">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" s="23"/>
+      <c r="L17" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25"/>
+      <c r="C18" s="21">
+        <v>4</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="21">
+        <v>5</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="21">
+        <v>6</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="21">
+        <v>7</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="21">
+        <v>8</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="21">
+        <v>9</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
+      <c r="C24" s="21">
+        <v>10</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="23"/>
+      <c r="L24" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="P24" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q24" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="R24" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E52" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E53" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E54" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E55" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E56" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E59" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E60" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E61" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E64" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E65" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E66" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E67" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E68" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E69" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E70" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E71" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E72" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E73" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="D2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>